<commit_message>
doing all model creations
</commit_message>
<xml_diff>
--- a/AnalysisDocumentnew.xlsx
+++ b/AnalysisDocumentnew.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B44B99-0CB4-4045-A27C-B3256DE46EF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644F851F-4C70-4E40-95EF-A575064708FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" tabRatio="675" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainScenarios" sheetId="1" r:id="rId1"/>
@@ -470,9 +470,6 @@
     <t>When a quote is being created a notification need to send to the manager</t>
   </si>
   <si>
-    <t>Messages</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -804,13 +801,16 @@
   </si>
   <si>
     <t>ModelId</t>
+  </si>
+  <si>
+    <t>SystemMessages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -879,14 +879,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -895,6 +887,22 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1014,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1042,19 +1050,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1069,6 +1076,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,12 +1401,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="108.125" customWidth="1"/>
+    <col min="2" max="2" width="108.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="48.95" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1413,7 +1422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="81.55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1429,207 +1438,207 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="97.85" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="97.9" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="12"/>
     </row>
-    <row r="7" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="12"/>
     </row>
-    <row r="8" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
     </row>
-    <row r="9" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
     </row>
-    <row r="12" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>37</v>
       </c>
@@ -1649,10 +1658,10 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.125" customWidth="1"/>
-    <col min="3" max="3" width="51.5" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -1672,15 +1681,15 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
         <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1696,9 +1705,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="146.25" customWidth="1"/>
+    <col min="2" max="2" width="146.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1730,12 +1739,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="99.25" customWidth="1"/>
+    <col min="2" max="2" width="99.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1759,211 +1768,211 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="12"/>
     </row>
-    <row r="5" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="12"/>
     </row>
-    <row r="6" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="12"/>
     </row>
-    <row r="7" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="12"/>
     </row>
-    <row r="8" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
     </row>
-    <row r="9" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
     </row>
-    <row r="12" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>37</v>
       </c>
@@ -1982,12 +1991,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="127.625" customWidth="1"/>
+    <col min="2" max="2" width="127.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="48.95" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2003,7 +2012,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2027,7 +2036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2035,7 +2044,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2043,7 +2052,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2059,7 +2068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="48.95" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2067,7 +2076,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2075,7 +2084,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2083,190 +2092,190 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="12"/>
     </row>
-    <row r="39" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="13"/>
     </row>
-    <row r="40" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="13"/>
     </row>
-    <row r="41" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
     </row>
-    <row r="42" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
     </row>
-    <row r="43" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="9"/>
     </row>
-    <row r="44" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
     </row>
-    <row r="45" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
     </row>
-    <row r="46" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
     </row>
   </sheetData>
@@ -2282,12 +2291,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="120.125" customWidth="1"/>
+    <col min="2" max="2" width="120.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2319,217 +2328,217 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
     </row>
-    <row r="12" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>37</v>
       </c>
@@ -2548,12 +2557,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="104" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>45</v>
       </c>
@@ -2569,7 +2578,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="32.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="32.65" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2585,211 +2594,211 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
     </row>
-    <row r="9" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
     </row>
-    <row r="12" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>37</v>
       </c>
@@ -2808,12 +2817,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="85.125" customWidth="1"/>
+    <col min="2" max="2" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2821,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48.9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="48.95" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2829,7 +2838,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2837,7 +2846,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2845,211 +2854,211 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
     </row>
-    <row r="9" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="12"/>
     </row>
-    <row r="12" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="12"/>
     </row>
-    <row r="16" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="12"/>
     </row>
-    <row r="27" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="12"/>
     </row>
-    <row r="30" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="12"/>
     </row>
-    <row r="33" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="12"/>
     </row>
-    <row r="34" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="12"/>
     </row>
-    <row r="35" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="12"/>
     </row>
-    <row r="38" spans="1:2" ht="16.3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3067,34 +3076,34 @@
   </sheetPr>
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
-    <col min="2" max="2" width="26.625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="5.375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.75" customWidth="1"/>
-    <col min="11" max="11" width="16.25" customWidth="1"/>
-    <col min="13" max="13" width="12.875" customWidth="1"/>
-    <col min="14" max="14" width="13.25" customWidth="1"/>
-    <col min="15" max="15" width="11.375" customWidth="1"/>
-    <col min="16" max="16" width="13.25" customWidth="1"/>
-    <col min="17" max="17" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.75" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>46</v>
       </c>
@@ -3102,87 +3111,87 @@
         <v>8</v>
       </c>
       <c r="C1" s="8"/>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="33"/>
-    </row>
-    <row r="2" spans="1:27" ht="19.05" x14ac:dyDescent="0.35">
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="32"/>
+    </row>
+    <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="I2" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="21" t="s">
         <v>21</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="S2" s="20"/>
+      <c r="R2" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" s="19"/>
       <c r="T2" s="17"/>
       <c r="U2" s="17"/>
       <c r="V2" s="17"/>
@@ -3192,58 +3201,58 @@
       <c r="Z2" s="17"/>
       <c r="AA2" s="18"/>
     </row>
-    <row r="3" spans="1:27" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D3" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="28" t="s">
-        <v>211</v>
+      <c r="Q3" s="27" t="s">
+        <v>210</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S3" t="s">
         <v>24</v>
@@ -3261,21 +3270,21 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -3289,41 +3298,41 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="34" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D5" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="K5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -3340,46 +3349,46 @@
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D6" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="N6" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="O6" s="26" t="s">
+      <c r="O6" s="25" t="s">
         <v>58</v>
       </c>
       <c r="P6" s="15" t="s">
@@ -3398,7 +3407,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
@@ -3407,31 +3416,31 @@
       <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="34" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D7" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -3445,41 +3454,41 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="34" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D8" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -3493,29 +3502,29 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="34" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D9" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -3529,35 +3538,35 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -3571,33 +3580,33 @@
       <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="34" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -3611,29 +3620,29 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="34" t="s">
         <v>89</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -3647,33 +3656,33 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="34" t="s">
         <v>92</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D13" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -3687,35 +3696,35 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="34" t="s">
         <v>96</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D14" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -3729,31 +3738,31 @@
       <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="34" t="s">
         <v>99</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D15" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -3766,38 +3775,38 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>105</v>
+        <v>216</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="22" t="s">
+      <c r="F16" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="H16" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
+      <c r="I16" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -3810,32 +3819,32 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="E17" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -3848,36 +3857,36 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="H18" s="22" t="s">
+      <c r="G18" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="H18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -3890,48 +3899,48 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D19" s="22" t="s">
+      <c r="E19" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="22" t="s">
+      <c r="H19" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="H19" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="22" t="s">
+      <c r="J19" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="M19" s="22" t="s">
+      <c r="L19" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="N19" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -3944,32 +3953,32 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="22" t="s">
+      <c r="F20" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -3982,26 +3991,26 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -4014,26 +4023,26 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -4046,44 +4055,44 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="28" t="s">
+      <c r="F23" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I23" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="H23" s="22" t="s">
+      <c r="J23" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="L23" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="L23" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -4096,26 +4105,26 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -4128,26 +4137,26 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
+        <v>202</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -4160,30 +4169,30 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D26" s="22" t="s">
+      <c r="E26" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
@@ -4196,38 +4205,38 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D27" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="H27" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="I27" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="I27" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -4240,36 +4249,36 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="H28" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
@@ -4282,32 +4291,32 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -4320,34 +4329,34 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E30" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="F30" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
+      <c r="G30" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
@@ -4360,36 +4369,36 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" s="22" t="s">
+      <c r="E31" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -4402,48 +4411,48 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="E32" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="G32" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="H32" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="I32" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="H32" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="I32" s="22" t="s">
+      <c r="J32" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="J32" s="22" t="s">
+      <c r="K32" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="K32" s="22" t="s">
+      <c r="L32" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="L32" s="22" t="s">
+      <c r="M32" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="N32" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="N32" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -4456,48 +4465,48 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D33" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="G33" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="H33" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="I33" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="H33" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="I33" s="22" t="s">
+      <c r="J33" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="J33" s="22" t="s">
+      <c r="K33" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="K33" s="22" t="s">
+      <c r="L33" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="L33" s="22" t="s">
+      <c r="M33" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="N33" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="N33" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -4510,48 +4519,48 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="22" t="s">
+      <c r="G34" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H34" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="G34" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="22" t="s">
+      <c r="I34" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="I34" s="22" t="s">
+      <c r="J34" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="J34" s="22" t="s">
+      <c r="K34" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L34" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="K34" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L34" s="22" t="s">
+      <c r="M34" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="N34" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="N34" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -4564,30 +4573,30 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -4600,34 +4609,34 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G36" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="G36" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
@@ -4640,44 +4649,44 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="22" t="s">
+      <c r="G37" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="G37" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-    </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+    </row>
+    <row r="38" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="16"/>
     </row>
@@ -4755,15 +4764,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.375" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4780,7 +4789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4793,7 +4802,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4802,7 +4811,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4811,7 +4820,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4820,7 +4829,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4829,7 +4838,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4838,7 +4847,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4847,7 +4856,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4856,7 +4865,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4865,7 +4874,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4874,7 +4883,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -4883,7 +4892,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -4892,7 +4901,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -4901,7 +4910,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -4910,7 +4919,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -4919,7 +4928,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -4928,7 +4937,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -4937,7 +4946,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -4946,7 +4955,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -4955,7 +4964,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -4964,7 +4973,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -4973,7 +4982,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -4982,7 +4991,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -4991,7 +5000,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -5000,7 +5009,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -5009,7 +5018,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -5018,7 +5027,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -5027,7 +5036,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5036,7 +5045,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5045,7 +5054,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5054,7 +5063,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5063,7 +5072,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5072,7 +5081,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5081,7 +5090,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5090,7 +5099,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5099,7 +5108,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5108,7 +5117,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5130,15 +5139,15 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.375" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5155,7 +5164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5164,7 +5173,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5173,7 +5182,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5182,7 +5191,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5191,7 +5200,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5200,7 +5209,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5209,7 +5218,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5218,7 +5227,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5227,7 +5236,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -5236,7 +5245,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -5245,7 +5254,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -5254,7 +5263,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5263,7 +5272,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5272,7 +5281,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5281,7 +5290,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -5290,7 +5299,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -5299,7 +5308,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -5308,7 +5317,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -5317,7 +5326,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -5326,7 +5335,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -5335,7 +5344,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -5344,7 +5353,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -5353,7 +5362,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -5362,7 +5371,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -5371,7 +5380,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -5380,7 +5389,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -5389,7 +5398,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -5398,7 +5407,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -5407,7 +5416,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -5416,7 +5425,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -5425,7 +5434,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -5434,7 +5443,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -5443,7 +5452,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -5452,7 +5461,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -5461,7 +5470,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -5470,7 +5479,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -5479,7 +5488,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
doing all model creations 2
</commit_message>
<xml_diff>
--- a/AnalysisDocumentnew.xlsx
+++ b/AnalysisDocumentnew.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644F851F-4C70-4E40-95EF-A575064708FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7FE8DB-D762-4397-B325-10261E259F72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainScenarios" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="218">
   <si>
     <t>No</t>
   </si>
@@ -470,9 +470,6 @@
     <t>When a quote is being created a notification need to send to the manager</t>
   </si>
   <si>
-    <t>Tasks</t>
-  </si>
-  <si>
     <t>Caption</t>
   </si>
   <si>
@@ -804,6 +801,12 @@
   </si>
   <si>
     <t>SystemMessages</t>
+  </si>
+  <si>
+    <t>SystemTasks</t>
+  </si>
+  <si>
+    <t>ClickedId</t>
   </si>
 </sst>
 </file>
@@ -1443,7 +1446,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -1681,15 +1684,15 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
         <v>117</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2100,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2105,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2333,7 +2336,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2341,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2349,7 +2352,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2357,7 +2360,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2365,7 +2368,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2373,7 +2376,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2599,7 +2602,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2607,7 +2610,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2615,7 +2618,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2859,7 +2862,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2867,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -2875,7 +2878,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.350000000000001" x14ac:dyDescent="0.3">
@@ -3077,7 +3080,7 @@
   <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D33" sqref="D33:N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,28 +3144,28 @@
     <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="H2" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="I2" s="28" t="s">
         <v>208</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>209</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>29</v>
@@ -3189,7 +3192,7 @@
         <v>22</v>
       </c>
       <c r="R2" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S2" s="19"/>
       <c r="T2" s="17"/>
@@ -3207,7 +3210,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>51</v>
@@ -3249,10 +3252,10 @@
         <v>30</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S3" t="s">
         <v>24</v>
@@ -3302,7 +3305,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>42</v>
@@ -3311,7 +3314,7 @@
         <v>43</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>44</v>
@@ -3326,7 +3329,7 @@
         <v>48</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
@@ -3353,16 +3356,16 @@
         <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>215</v>
-      </c>
       <c r="F6" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>44</v>
@@ -3377,16 +3380,16 @@
         <v>48</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L6" s="22" t="s">
         <v>50</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O6" s="25" t="s">
         <v>58</v>
@@ -3407,7 +3410,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
@@ -3420,7 +3423,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>50</v>
@@ -3458,7 +3461,7 @@
         <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>50</v>
@@ -3506,7 +3509,7 @@
         <v>82</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>80</v>
@@ -3542,7 +3545,7 @@
         <v>86</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>80</v>
@@ -3584,7 +3587,7 @@
         <v>87</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>80</v>
@@ -3624,7 +3627,7 @@
         <v>89</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>80</v>
@@ -3660,7 +3663,7 @@
         <v>92</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>80</v>
@@ -3700,7 +3703,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>80</v>
@@ -3742,7 +3745,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>50</v>
@@ -3775,30 +3778,30 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>216</v>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>215</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="H16" s="21" t="s">
-        <v>144</v>
-      </c>
       <c r="I16" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
@@ -3819,21 +3822,21 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>105</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>106</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -3859,22 +3862,22 @@
     </row>
     <row r="18" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="21" t="s">
-        <v>130</v>
-      </c>
       <c r="G18" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>32</v>
@@ -3901,43 +3904,43 @@
     </row>
     <row r="19" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>112</v>
-      </c>
       <c r="E19" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F19" s="22" t="s">
         <v>50</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>55</v>
       </c>
       <c r="I19" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="J19" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>115</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>32</v>
       </c>
       <c r="L19" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M19" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="N19" s="21" t="s">
         <v>122</v>
-      </c>
-      <c r="N19" s="21" t="s">
-        <v>123</v>
       </c>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
@@ -3955,19 +3958,19 @@
     </row>
     <row r="20" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="21" t="s">
+      <c r="F20" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>121</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
@@ -3993,10 +3996,10 @@
     </row>
     <row r="21" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -4025,10 +4028,10 @@
     </row>
     <row r="22" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -4057,37 +4060,37 @@
     </row>
     <row r="23" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>50</v>
       </c>
       <c r="G23" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="21" t="s">
-        <v>135</v>
-      </c>
       <c r="I23" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J23" s="21" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
@@ -4107,10 +4110,10 @@
     </row>
     <row r="24" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -4139,10 +4142,10 @@
     </row>
     <row r="25" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -4171,16 +4174,16 @@
     </row>
     <row r="26" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D26" s="21" t="s">
+      <c r="E26" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>147</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -4205,30 +4208,30 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>156</v>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B27" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>50</v>
+        <v>217</v>
       </c>
       <c r="F27" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="H27" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="I27" s="21" t="s">
         <v>154</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>155</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
@@ -4249,27 +4252,27 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>157</v>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
+        <v>156</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>50</v>
       </c>
       <c r="E28" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>153</v>
-      </c>
       <c r="G28" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="20"/>
@@ -4293,19 +4296,19 @@
     </row>
     <row r="29" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>160</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>161</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
@@ -4331,22 +4334,22 @@
     </row>
     <row r="30" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E30" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>163</v>
-      </c>
       <c r="G30" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
@@ -4371,25 +4374,25 @@
     </row>
     <row r="31" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>165</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>166</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
@@ -4413,43 +4416,43 @@
     </row>
     <row r="32" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E32" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="G32" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="H32" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="I32" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H32" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="I32" s="21" t="s">
+      <c r="J32" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="J32" s="21" t="s">
+      <c r="K32" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="K32" s="21" t="s">
+      <c r="L32" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="L32" s="21" t="s">
+      <c r="M32" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="M32" s="21" t="s">
+      <c r="N32" s="21" t="s">
         <v>185</v>
-      </c>
-      <c r="N32" s="21" t="s">
-        <v>186</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
@@ -4465,45 +4468,45 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>187</v>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B33" s="34" t="s">
+        <v>186</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>50</v>
       </c>
       <c r="E33" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="G33" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="H33" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="I33" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H33" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="I33" s="21" t="s">
+      <c r="J33" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="K33" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="K33" s="21" t="s">
+      <c r="L33" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="L33" s="21" t="s">
+      <c r="M33" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="M33" s="21" t="s">
+      <c r="N33" s="21" t="s">
         <v>185</v>
-      </c>
-      <c r="N33" s="21" t="s">
-        <v>186</v>
       </c>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
@@ -4519,12 +4522,12 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>189</v>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B34" s="34" t="s">
+        <v>188</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>50</v>
@@ -4533,31 +4536,31 @@
         <v>51</v>
       </c>
       <c r="F34" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="G34" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H34" s="21" t="s">
+      <c r="I34" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="J34" s="21" t="s">
         <v>192</v>
-      </c>
-      <c r="J34" s="21" t="s">
-        <v>193</v>
       </c>
       <c r="K34" s="21" t="s">
         <v>58</v>
       </c>
       <c r="L34" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="M34" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="M34" s="21" t="s">
+      <c r="N34" s="21" t="s">
         <v>195</v>
-      </c>
-      <c r="N34" s="21" t="s">
-        <v>196</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
@@ -4575,13 +4578,13 @@
     </row>
     <row r="35" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E35" s="21" t="s">
         <v>97</v>
@@ -4611,22 +4614,22 @@
     </row>
     <row r="36" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E36" s="21" t="s">
         <v>15</v>
       </c>
       <c r="F36" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G36" s="21" t="s">
         <v>200</v>
-      </c>
-      <c r="G36" s="21" t="s">
-        <v>201</v>
       </c>
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
@@ -4651,22 +4654,22 @@
     </row>
     <row r="37" spans="2:27" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>15</v>
       </c>
       <c r="F37" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G37" s="21" t="s">
         <v>200</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>201</v>
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>

</xml_diff>